<commit_message>
implemented some command line arguments, refactored the mapping to jira issues, added the fix versions to the serializer
</commit_message>
<xml_diff>
--- a/src/test/java/de/adesso/excel2jira/excel/issues-examples.xlsx
+++ b/src/test/java/de/adesso/excel2jira/excel/issues-examples.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkrause\Desktop\excel2jira\excel2Jira\src\test\java\de\adesso\excel2jira\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atanasov\workspace\excel2Jira\src\test\java\de\adesso\excel2jira\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16344"/>
   </bookViews>
   <sheets>
     <sheet name="general_report" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Projekt</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>3 - leicht umgehbar</t>
-  </si>
-  <si>
-    <t>Hombergs, Tom</t>
   </si>
   <si>
     <t>Bitte das folgende Szenario evaluieren / ausprobieren: 
@@ -103,13 +100,13 @@
     <t>Standort 4711</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>eins, zwei</t>
   </si>
   <si>
     <t>eins</t>
+  </si>
+  <si>
+    <t>hombergs</t>
   </si>
 </sst>
 </file>
@@ -1000,24 +997,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="392" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="400.2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1051,30 +1048,30 @@
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>4711</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="124.2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -1083,24 +1080,24 @@
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>10</v>
@@ -1109,16 +1106,16 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added fixVersions and url command line arguments and refactored
</commit_message>
<xml_diff>
--- a/src/test/java/de/adesso/excel2jira/excel/issues-examples.xlsx
+++ b/src/test/java/de/adesso/excel2jira/excel/issues-examples.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Projekt</t>
   </si>
@@ -998,7 +998,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -1050,8 +1050,8 @@
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3">
-        <v>4711</v>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>22</v>

</xml_diff>